<commit_message>
feat: implemented import excel for updating status
</commit_message>
<xml_diff>
--- a/public/sample_updateStatus.xlsx
+++ b/public/sample_updateStatus.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\arjunv\work\Placify\Placify.io\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76F9719-80DE-4BA0-92C2-575C0ACF0366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>abc@sample.com</t>
+  </si>
+  <si>
+    <t>def@sample.com</t>
+  </si>
+  <si>
+    <t>efg@sample.com</t>
+  </si>
+  <si>
+    <t>ijk@sample.com</t>
+  </si>
+  <si>
+    <t>lmn@sample.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +86,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +373,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7C5FF7BF-E240-47A9-9F13-43625C9C79D7}"/>
+    <hyperlink ref="A3:A6" r:id="rId2" display="abc@sample.com" xr:uid="{5EEC542F-8996-414E-BE4E-B80D7B0DB5A2}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{4CBDB85D-78A6-48D1-9E13-8BFE94279A39}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{75FFB6B9-AF74-44DA-9BA1-EC0C3A266975}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{EC94E707-8605-4706-A454-B685363883D3}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{9CEC7115-854A-4B26-AE11-760AA90E5F7C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: added delete student
</commit_message>
<xml_diff>
--- a/public/sample_updateStatus.xlsx
+++ b/public/sample_updateStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\arjunv\work\Placify\Placify.io\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76F9719-80DE-4BA0-92C2-575C0ACF0366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC6D875-7380-491E-AFCB-A95DF0F3955A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
@@ -46,6 +46,30 @@
   </si>
   <si>
     <t>lmn@sample.com</t>
+  </si>
+  <si>
+    <t>studentID</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>contactNo</t>
+  </si>
+  <si>
+    <t>tenthMarks</t>
+  </si>
+  <si>
+    <t>twelthMarks</t>
+  </si>
+  <si>
+    <t>studentUGMarks</t>
+  </si>
+  <si>
+    <t>studentPGMarks</t>
+  </si>
+  <si>
+    <t>studentDescription</t>
   </si>
 </sst>
 </file>
@@ -374,70 +398,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="I3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="I4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="I5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="I6">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7C5FF7BF-E240-47A9-9F13-43625C9C79D7}"/>
-    <hyperlink ref="A3:A6" r:id="rId2" display="abc@sample.com" xr:uid="{5EEC542F-8996-414E-BE4E-B80D7B0DB5A2}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{4CBDB85D-78A6-48D1-9E13-8BFE94279A39}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{75FFB6B9-AF74-44DA-9BA1-EC0C3A266975}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{EC94E707-8605-4706-A454-B685363883D3}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{9CEC7115-854A-4B26-AE11-760AA90E5F7C}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{7C5FF7BF-E240-47A9-9F13-43625C9C79D7}"/>
+    <hyperlink ref="C3:C6" r:id="rId2" display="abc@sample.com" xr:uid="{5EEC542F-8996-414E-BE4E-B80D7B0DB5A2}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{4CBDB85D-78A6-48D1-9E13-8BFE94279A39}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{75FFB6B9-AF74-44DA-9BA1-EC0C3A266975}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{EC94E707-8605-4706-A454-B685363883D3}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{9CEC7115-854A-4B26-AE11-760AA90E5F7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>